<commit_message>
tried debugging multiple loco's => in search for working instances
</commit_message>
<xml_diff>
--- a/Task states.xlsx
+++ b/Task states.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="14">
   <si>
     <t>name</t>
   </si>
@@ -53,6 +53,9 @@
   </si>
   <si>
     <t>Pouring</t>
+  </si>
+  <si>
+    <t>-&gt; WZ</t>
   </si>
 </sst>
 </file>
@@ -410,7 +413,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E97"/>
+  <dimension ref="A1:E108"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -438,7 +441,7 @@
         <v>5</v>
       </c>
       <c r="B2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C2" t="b">
         <v>1</v>
@@ -455,13 +458,16 @@
         <v>6</v>
       </c>
       <c r="B3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C3" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>289</v>
       </c>
       <c r="E3">
-        <v>1498</v>
+        <v>288</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -469,13 +475,16 @@
         <v>7</v>
       </c>
       <c r="B4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C4" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>372</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>83</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -483,13 +492,16 @@
         <v>8</v>
       </c>
       <c r="B5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C5" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>417</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -497,13 +509,13 @@
         <v>9</v>
       </c>
       <c r="B6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C6" t="b">
         <v>0</v>
       </c>
       <c r="E6">
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -511,7 +523,7 @@
         <v>10</v>
       </c>
       <c r="B7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C7" t="b">
         <v>0</v>
@@ -525,7 +537,7 @@
         <v>11</v>
       </c>
       <c r="B8">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C8" t="b">
         <v>0</v>
@@ -539,7 +551,7 @@
         <v>12</v>
       </c>
       <c r="B9">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C9" t="b">
         <v>0</v>
@@ -550,38 +562,38 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B10">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C10" t="b">
-        <v>1</v>
-      </c>
-      <c r="D10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E10">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B11">
         <v>4</v>
       </c>
       <c r="C11" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
       </c>
       <c r="E11">
-        <v>1498</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B12">
         <v>4</v>
@@ -590,12 +602,12 @@
         <v>0</v>
       </c>
       <c r="E12">
-        <v>0</v>
+        <v>425</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B13">
         <v>4</v>
@@ -609,7 +621,7 @@
     </row>
     <row r="14" spans="1:5">
       <c r="A14" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B14">
         <v>4</v>
@@ -623,7 +635,7 @@
     </row>
     <row r="15" spans="1:5">
       <c r="A15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B15">
         <v>4</v>
@@ -637,7 +649,7 @@
     </row>
     <row r="16" spans="1:5">
       <c r="A16" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B16">
         <v>4</v>
@@ -651,7 +663,7 @@
     </row>
     <row r="17" spans="1:5">
       <c r="A17" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B17">
         <v>4</v>
@@ -665,41 +677,38 @@
     </row>
     <row r="18" spans="1:5">
       <c r="A18" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="B18">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C18" t="b">
-        <v>1</v>
-      </c>
-      <c r="D18">
-        <v>538</v>
+        <v>0</v>
       </c>
       <c r="E18">
-        <v>538</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B19">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C19" t="b">
         <v>0</v>
       </c>
       <c r="E19">
-        <v>961</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B20">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C20" t="b">
         <v>0</v>
@@ -710,10 +719,10 @@
     </row>
     <row r="21" spans="1:5">
       <c r="A21" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B21">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C21" t="b">
         <v>0</v>
@@ -724,10 +733,10 @@
     </row>
     <row r="22" spans="1:5">
       <c r="A22" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B22">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C22" t="b">
         <v>0</v>
@@ -738,10 +747,10 @@
     </row>
     <row r="23" spans="1:5">
       <c r="A23" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B23">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C23" t="b">
         <v>0</v>
@@ -752,10 +761,10 @@
     </row>
     <row r="24" spans="1:5">
       <c r="A24" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B24">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C24" t="b">
         <v>0</v>
@@ -766,10 +775,10 @@
     </row>
     <row r="25" spans="1:5">
       <c r="A25" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B25">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C25" t="b">
         <v>0</v>
@@ -780,194 +789,164 @@
     </row>
     <row r="26" spans="1:5">
       <c r="A26" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="B26">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C26" t="b">
-        <v>1</v>
-      </c>
-      <c r="D26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E26">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="B27">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C27" t="b">
-        <v>1</v>
-      </c>
-      <c r="D27">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="E27">
-        <v>18</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B28">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C28" t="b">
         <v>1</v>
       </c>
       <c r="D28">
-        <v>192</v>
+        <v>1</v>
       </c>
       <c r="E28">
-        <v>173</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B29">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C29" t="b">
-        <v>1</v>
-      </c>
-      <c r="D29">
-        <v>237</v>
+        <v>0</v>
       </c>
       <c r="E29">
-        <v>45</v>
+        <v>425</v>
       </c>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B30">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C30" t="b">
-        <v>1</v>
-      </c>
-      <c r="D30">
-        <v>291</v>
+        <v>0</v>
       </c>
       <c r="E30">
-        <v>54</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B31">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C31" t="b">
-        <v>1</v>
-      </c>
-      <c r="D31">
-        <v>380</v>
+        <v>0</v>
       </c>
       <c r="E31">
-        <v>89</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:5">
       <c r="A32" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B32">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C32" t="b">
-        <v>1</v>
-      </c>
-      <c r="D32">
-        <v>456</v>
+        <v>0</v>
       </c>
       <c r="E32">
-        <v>76</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:5">
       <c r="A33" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B33">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C33" t="b">
-        <v>1</v>
-      </c>
-      <c r="D33">
-        <v>479</v>
+        <v>0</v>
       </c>
       <c r="E33">
-        <v>23</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:5">
       <c r="A34" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B34">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C34" t="b">
-        <v>1</v>
-      </c>
-      <c r="D34">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E34">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:5">
       <c r="A35" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B35">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C35" t="b">
-        <v>1</v>
-      </c>
-      <c r="D35">
-        <v>204</v>
+        <v>0</v>
       </c>
       <c r="E35">
-        <v>203</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:5">
       <c r="A36" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="B36">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C36" t="b">
-        <v>1</v>
-      </c>
-      <c r="D36">
-        <v>473</v>
+        <v>0</v>
       </c>
       <c r="E36">
-        <v>269</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:5">
       <c r="A37" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B37">
         <v>10</v>
@@ -976,151 +955,127 @@
         <v>1</v>
       </c>
       <c r="D37">
-        <v>518</v>
+        <v>1</v>
       </c>
       <c r="E37">
-        <v>45</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:5">
       <c r="A38" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B38">
         <v>10</v>
       </c>
       <c r="C38" t="b">
-        <v>1</v>
-      </c>
-      <c r="D38">
-        <v>678</v>
+        <v>0</v>
       </c>
       <c r="E38">
-        <v>160</v>
+        <v>425</v>
       </c>
     </row>
     <row r="39" spans="1:5">
       <c r="A39" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B39">
         <v>10</v>
       </c>
       <c r="C39" t="b">
-        <v>1</v>
-      </c>
-      <c r="D39">
-        <v>950</v>
+        <v>0</v>
       </c>
       <c r="E39">
-        <v>272</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:5">
       <c r="A40" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B40">
         <v>10</v>
       </c>
       <c r="C40" t="b">
-        <v>1</v>
-      </c>
-      <c r="D40">
-        <v>1026</v>
+        <v>0</v>
       </c>
       <c r="E40">
-        <v>76</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:5">
       <c r="A41" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B41">
         <v>10</v>
       </c>
       <c r="C41" t="b">
-        <v>1</v>
-      </c>
-      <c r="D41">
-        <v>1054</v>
+        <v>0</v>
       </c>
       <c r="E41">
-        <v>28</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:5">
       <c r="A42" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B42">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C42" t="b">
-        <v>1</v>
-      </c>
-      <c r="D42">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E42">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:5">
       <c r="A43" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B43">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C43" t="b">
-        <v>1</v>
-      </c>
-      <c r="D43">
-        <v>1063</v>
+        <v>0</v>
       </c>
       <c r="E43">
-        <v>1062</v>
+        <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:5">
       <c r="A44" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="B44">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C44" t="b">
-        <v>1</v>
-      </c>
-      <c r="D44">
-        <v>1157</v>
+        <v>0</v>
       </c>
       <c r="E44">
-        <v>94</v>
+        <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:5">
       <c r="A45" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="B45">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C45" t="b">
-        <v>1</v>
-      </c>
-      <c r="D45">
-        <v>1202</v>
+        <v>0</v>
       </c>
       <c r="E45">
-        <v>45</v>
+        <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:5">
       <c r="A46" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B46">
         <v>11</v>
@@ -1129,29 +1084,32 @@
         <v>1</v>
       </c>
       <c r="D46">
-        <v>1446</v>
+        <v>1</v>
       </c>
       <c r="E46">
-        <v>244</v>
+        <v>1</v>
       </c>
     </row>
     <row r="47" spans="1:5">
       <c r="A47" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B47">
         <v>11</v>
       </c>
       <c r="C47" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="D47">
+        <v>377</v>
       </c>
       <c r="E47">
-        <v>53</v>
+        <v>376</v>
       </c>
     </row>
     <row r="48" spans="1:5">
       <c r="A48" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B48">
         <v>11</v>
@@ -1160,12 +1118,12 @@
         <v>0</v>
       </c>
       <c r="E48">
-        <v>0</v>
+        <v>49</v>
       </c>
     </row>
     <row r="49" spans="1:5">
       <c r="A49" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B49">
         <v>11</v>
@@ -1179,58 +1137,52 @@
     </row>
     <row r="50" spans="1:5">
       <c r="A50" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B50">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C50" t="b">
-        <v>1</v>
-      </c>
-      <c r="D50">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E50">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:5">
       <c r="A51" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B51">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C51" t="b">
-        <v>1</v>
-      </c>
-      <c r="D51">
-        <v>1253</v>
+        <v>0</v>
       </c>
       <c r="E51">
-        <v>1252</v>
+        <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:5">
       <c r="A52" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B52">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C52" t="b">
         <v>0</v>
       </c>
       <c r="E52">
-        <v>246</v>
+        <v>0</v>
       </c>
     </row>
     <row r="53" spans="1:5">
       <c r="A53" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B53">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C53" t="b">
         <v>0</v>
@@ -1241,10 +1193,10 @@
     </row>
     <row r="54" spans="1:5">
       <c r="A54" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B54">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C54" t="b">
         <v>0</v>
@@ -1255,7 +1207,7 @@
     </row>
     <row r="55" spans="1:5">
       <c r="A55" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B55">
         <v>12</v>
@@ -1264,12 +1216,12 @@
         <v>0</v>
       </c>
       <c r="E55">
-        <v>0</v>
+        <v>426</v>
       </c>
     </row>
     <row r="56" spans="1:5">
       <c r="A56" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B56">
         <v>12</v>
@@ -1283,7 +1235,7 @@
     </row>
     <row r="57" spans="1:5">
       <c r="A57" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B57">
         <v>12</v>
@@ -1297,151 +1249,139 @@
     </row>
     <row r="58" spans="1:5">
       <c r="A58" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B58">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C58" t="b">
-        <v>1</v>
-      </c>
-      <c r="D58">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E58">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="59" spans="1:5">
       <c r="A59" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B59">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C59" t="b">
-        <v>1</v>
-      </c>
-      <c r="D59">
-        <v>339</v>
+        <v>0</v>
       </c>
       <c r="E59">
-        <v>338</v>
+        <v>0</v>
       </c>
     </row>
     <row r="60" spans="1:5">
       <c r="A60" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B60">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C60" t="b">
-        <v>1</v>
-      </c>
-      <c r="D60">
-        <v>648</v>
+        <v>0</v>
       </c>
       <c r="E60">
-        <v>309</v>
+        <v>0</v>
       </c>
     </row>
     <row r="61" spans="1:5">
       <c r="A61" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B61">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C61" t="b">
-        <v>1</v>
-      </c>
-      <c r="D61">
-        <v>693</v>
+        <v>0</v>
       </c>
       <c r="E61">
-        <v>45</v>
+        <v>0</v>
       </c>
     </row>
     <row r="62" spans="1:5">
       <c r="A62" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B62">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C62" t="b">
-        <v>1</v>
-      </c>
-      <c r="D62">
-        <v>796</v>
+        <v>0</v>
       </c>
       <c r="E62">
-        <v>103</v>
+        <v>0</v>
       </c>
     </row>
     <row r="63" spans="1:5">
       <c r="A63" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B63">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C63" t="b">
         <v>0</v>
       </c>
       <c r="E63">
-        <v>703</v>
+        <v>0</v>
       </c>
     </row>
     <row r="64" spans="1:5">
       <c r="A64" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B64">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="C64" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="D64">
+        <v>1</v>
       </c>
       <c r="E64">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="65" spans="1:5">
       <c r="A65" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B65">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="C65" t="b">
         <v>0</v>
       </c>
       <c r="E65">
-        <v>0</v>
+        <v>425</v>
       </c>
     </row>
     <row r="66" spans="1:5">
       <c r="A66" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B66">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="C66" t="b">
         <v>0</v>
       </c>
       <c r="E66">
-        <v>1499</v>
+        <v>0</v>
       </c>
     </row>
     <row r="67" spans="1:5">
       <c r="A67" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B67">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="C67" t="b">
         <v>0</v>
@@ -1452,10 +1392,10 @@
     </row>
     <row r="68" spans="1:5">
       <c r="A68" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B68">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="C68" t="b">
         <v>0</v>
@@ -1466,10 +1406,10 @@
     </row>
     <row r="69" spans="1:5">
       <c r="A69" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B69">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="C69" t="b">
         <v>0</v>
@@ -1480,10 +1420,10 @@
     </row>
     <row r="70" spans="1:5">
       <c r="A70" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B70">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="C70" t="b">
         <v>0</v>
@@ -1494,10 +1434,10 @@
     </row>
     <row r="71" spans="1:5">
       <c r="A71" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B71">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="C71" t="b">
         <v>0</v>
@@ -1508,10 +1448,10 @@
     </row>
     <row r="72" spans="1:5">
       <c r="A72" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B72">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="C72" t="b">
         <v>0</v>
@@ -1522,55 +1462,55 @@
     </row>
     <row r="73" spans="1:5">
       <c r="A73" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="B73">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="C73" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="D73">
+        <v>1</v>
       </c>
       <c r="E73">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="74" spans="1:5">
       <c r="A74" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B74">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C74" t="b">
-        <v>1</v>
-      </c>
-      <c r="D74">
-        <v>877</v>
+        <v>0</v>
       </c>
       <c r="E74">
-        <v>877</v>
+        <v>425</v>
       </c>
     </row>
     <row r="75" spans="1:5">
       <c r="A75" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B75">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C75" t="b">
         <v>0</v>
       </c>
       <c r="E75">
-        <v>622</v>
+        <v>0</v>
       </c>
     </row>
     <row r="76" spans="1:5">
       <c r="A76" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B76">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C76" t="b">
         <v>0</v>
@@ -1581,10 +1521,10 @@
     </row>
     <row r="77" spans="1:5">
       <c r="A77" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B77">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C77" t="b">
         <v>0</v>
@@ -1595,10 +1535,10 @@
     </row>
     <row r="78" spans="1:5">
       <c r="A78" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B78">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C78" t="b">
         <v>0</v>
@@ -1609,10 +1549,10 @@
     </row>
     <row r="79" spans="1:5">
       <c r="A79" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B79">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C79" t="b">
         <v>0</v>
@@ -1623,10 +1563,10 @@
     </row>
     <row r="80" spans="1:5">
       <c r="A80" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B80">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C80" t="b">
         <v>0</v>
@@ -1637,10 +1577,10 @@
     </row>
     <row r="81" spans="1:5">
       <c r="A81" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B81">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C81" t="b">
         <v>0</v>
@@ -1654,7 +1594,7 @@
         <v>5</v>
       </c>
       <c r="B82">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C82" t="b">
         <v>1</v>
@@ -1671,16 +1611,13 @@
         <v>6</v>
       </c>
       <c r="B83">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C83" t="b">
-        <v>1</v>
-      </c>
-      <c r="D83">
-        <v>617</v>
+        <v>0</v>
       </c>
       <c r="E83">
-        <v>616</v>
+        <v>425</v>
       </c>
     </row>
     <row r="84" spans="1:5">
@@ -1688,13 +1625,13 @@
         <v>7</v>
       </c>
       <c r="B84">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C84" t="b">
         <v>0</v>
       </c>
       <c r="E84">
-        <v>882</v>
+        <v>0</v>
       </c>
     </row>
     <row r="85" spans="1:5">
@@ -1702,7 +1639,7 @@
         <v>8</v>
       </c>
       <c r="B85">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C85" t="b">
         <v>0</v>
@@ -1716,7 +1653,7 @@
         <v>9</v>
       </c>
       <c r="B86">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C86" t="b">
         <v>0</v>
@@ -1730,7 +1667,7 @@
         <v>10</v>
       </c>
       <c r="B87">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C87" t="b">
         <v>0</v>
@@ -1744,7 +1681,7 @@
         <v>11</v>
       </c>
       <c r="B88">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C88" t="b">
         <v>0</v>
@@ -1758,7 +1695,7 @@
         <v>12</v>
       </c>
       <c r="B89">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C89" t="b">
         <v>0</v>
@@ -1769,38 +1706,38 @@
     </row>
     <row r="90" spans="1:5">
       <c r="A90" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B90">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C90" t="b">
         <v>0</v>
       </c>
       <c r="E90">
-        <v>1499</v>
+        <v>0</v>
       </c>
     </row>
     <row r="91" spans="1:5">
       <c r="A91" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B91">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C91" t="b">
         <v>0</v>
       </c>
       <c r="E91">
-        <v>0</v>
+        <v>426</v>
       </c>
     </row>
     <row r="92" spans="1:5">
       <c r="A92" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B92">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C92" t="b">
         <v>0</v>
@@ -1811,10 +1748,10 @@
     </row>
     <row r="93" spans="1:5">
       <c r="A93" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B93">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C93" t="b">
         <v>0</v>
@@ -1825,10 +1762,10 @@
     </row>
     <row r="94" spans="1:5">
       <c r="A94" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B94">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C94" t="b">
         <v>0</v>
@@ -1839,10 +1776,10 @@
     </row>
     <row r="95" spans="1:5">
       <c r="A95" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B95">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C95" t="b">
         <v>0</v>
@@ -1853,10 +1790,10 @@
     </row>
     <row r="96" spans="1:5">
       <c r="A96" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B96">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C96" t="b">
         <v>0</v>
@@ -1867,15 +1804,169 @@
     </row>
     <row r="97" spans="1:5">
       <c r="A97" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B97">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C97" t="b">
         <v>0</v>
       </c>
       <c r="E97">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5">
+      <c r="A98" t="s">
+        <v>12</v>
+      </c>
+      <c r="B98">
+        <v>25</v>
+      </c>
+      <c r="C98" t="b">
+        <v>0</v>
+      </c>
+      <c r="E98">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5">
+      <c r="A99" t="s">
+        <v>13</v>
+      </c>
+      <c r="B99">
+        <v>25</v>
+      </c>
+      <c r="C99" t="b">
+        <v>0</v>
+      </c>
+      <c r="E99">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5">
+      <c r="A100" t="s">
+        <v>5</v>
+      </c>
+      <c r="B100">
+        <v>27</v>
+      </c>
+      <c r="C100" t="b">
+        <v>0</v>
+      </c>
+      <c r="E100">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5">
+      <c r="A101" t="s">
+        <v>6</v>
+      </c>
+      <c r="B101">
+        <v>27</v>
+      </c>
+      <c r="C101" t="b">
+        <v>0</v>
+      </c>
+      <c r="E101">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5">
+      <c r="A102" t="s">
+        <v>7</v>
+      </c>
+      <c r="B102">
+        <v>27</v>
+      </c>
+      <c r="C102" t="b">
+        <v>0</v>
+      </c>
+      <c r="E102">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5">
+      <c r="A103" t="s">
+        <v>8</v>
+      </c>
+      <c r="B103">
+        <v>27</v>
+      </c>
+      <c r="C103" t="b">
+        <v>0</v>
+      </c>
+      <c r="E103">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5">
+      <c r="A104" t="s">
+        <v>9</v>
+      </c>
+      <c r="B104">
+        <v>27</v>
+      </c>
+      <c r="C104" t="b">
+        <v>0</v>
+      </c>
+      <c r="E104">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5">
+      <c r="A105" t="s">
+        <v>10</v>
+      </c>
+      <c r="B105">
+        <v>27</v>
+      </c>
+      <c r="C105" t="b">
+        <v>0</v>
+      </c>
+      <c r="E105">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5">
+      <c r="A106" t="s">
+        <v>11</v>
+      </c>
+      <c r="B106">
+        <v>27</v>
+      </c>
+      <c r="C106" t="b">
+        <v>0</v>
+      </c>
+      <c r="E106">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5">
+      <c r="A107" t="s">
+        <v>12</v>
+      </c>
+      <c r="B107">
+        <v>27</v>
+      </c>
+      <c r="C107" t="b">
+        <v>0</v>
+      </c>
+      <c r="E107">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5">
+      <c r="A108" t="s">
+        <v>13</v>
+      </c>
+      <c r="B108">
+        <v>27</v>
+      </c>
+      <c r="C108" t="b">
+        <v>0</v>
+      </c>
+      <c r="E108">
         <v>0</v>
       </c>
     </row>

</xml_diff>